<commit_message>
finished report and ppt
</commit_message>
<xml_diff>
--- a/outputs/results.xlsx
+++ b/outputs/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyas/Desktop/Workspace/FastStream Tech/ectm/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{010903D9-8A4E-DA4E-987B-564991421EA3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5106ABE7-31BD-9242-B8B2-D1E0C8668870}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{551CB910-A9A8-CB40-BF6B-D42A12EA74E9}"/>
   </bookViews>
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C32432-57A1-9C4E-B6EF-935570A417AE}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="262" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="244" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -417,7 +417,7 @@
     <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -444,8 +444,17 @@
       <c r="D3" s="2">
         <v>0.97819999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -458,8 +467,17 @@
       <c r="D4" s="2">
         <v>0.99590000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -472,8 +490,17 @@
       <c r="D5" s="2">
         <v>0.97989999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -486,8 +513,17 @@
       <c r="D6" s="2">
         <v>0.75480000000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -500,8 +536,17 @@
       <c r="D7" s="2">
         <v>0.99829999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -514,8 +559,17 @@
       <c r="D8" s="2">
         <v>0.90490000000000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -528,8 +582,17 @@
       <c r="D9" s="2">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -542,8 +605,17 @@
       <c r="D10" s="2">
         <v>0.95369999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -556,8 +628,17 @@
       <c r="D11" s="2">
         <v>0.8891</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -569,6 +650,38 @@
       </c>
       <c r="D12" s="2">
         <v>0.93579999999999997</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="2">
+        <f>SUM(B3:B12)</f>
+        <v>9.1145999999999994</v>
+      </c>
+      <c r="C13" s="2">
+        <f>SUM(C3:C12)</f>
+        <v>9.5964999999999989</v>
+      </c>
+      <c r="D13" s="2">
+        <f>SUM(D3:D12)</f>
+        <v>9.3806000000000012</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>